<commit_message>
logicComparator.py code now works on all the eligibility files. The exception is the hemoglobin trials which has a conditional code I'm not sure what to do with.
</commit_message>
<xml_diff>
--- a/SMC Challenge 6/eligibility criteria/Dataset1_HIV_Trials_First.xlsx
+++ b/SMC Challenge 6/eligibility criteria/Dataset1_HIV_Trials_First.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miste\PycharmProjects\ClinicalTrialChallenge\SMC Challenge 6\eligibility criteria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB059A3-6CAF-453D-8350-612FE39DBE69}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A106DA4-1676-4B08-94B4-1F11075F3A77}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1713" uniqueCount="1303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1713" uniqueCount="1302">
   <si>
     <t>official_title</t>
   </si>
@@ -3984,9 +3984,6 @@
     <t>(C15175=0) or (C15175=C17998) or (C15175=1 and C103810&gt;=350)</t>
   </si>
   <si>
-    <t>(C15175=0) or (C15175=C17998) or (C15175=1 and C103810&gt;499 and C92544&lt;50 {copies}/ml)</t>
-  </si>
-  <si>
     <t>(C15175=0)  or (C15175=C17998) or (C15175=1 and C103810&gt;350)</t>
   </si>
   <si>
@@ -3999,9 +3996,6 @@
     <t>(C15175=0) or (C15175=C17998) or (C15175=1 and C94631=0 and  C103810&gt;500)</t>
   </si>
   <si>
-    <t>C15175=0 or C15175=C17998 or (C15175=1 and  C103810&gt;=200) and C94631=1)</t>
-  </si>
-  <si>
     <t>C15175=0 or C15175=C17998 or (C15175=1 and C94631=0) or (C15175=1 and C94631=1 and  C103810&gt;C25555)</t>
   </si>
   <si>
@@ -4053,12 +4047,6 @@
     <t>C15175=0 or C15175=C17998 or (C15175=1 and (C94631=1) and C92544=C111568)</t>
   </si>
   <si>
-    <t>C15175=0 or C15175=C17998 or (C15175=1 and C103810&gt;=350 and C92544&lt;25000 and (C94631=1)</t>
-  </si>
-  <si>
-    <t>C15175=0 or C15175=C17998 or C2851=0 or C2851=C17998 or (C15175=1 and C103810&gt;=250 and C92544=C111568</t>
-  </si>
-  <si>
     <t>C15175=0 or C15175=C17998 or (C15175=1 and C103810&gt;350 and C92544=C111568 and C15840=0)</t>
   </si>
   <si>
@@ -4068,15 +4056,6 @@
     <t xml:space="preserve">(C15175=0 or C15175=C17998) </t>
   </si>
   <si>
-    <t>(C15175=0) or (C15175=C17998) or C15175=1 and C94631=0) or (C15175=1 and C2851=0)</t>
-  </si>
-  <si>
-    <t>(C15175=0) or (C15175=C17998) or (C15175 =1 and C94631=0) or (C15175=1 and C94631=1 and C111373=0 and  C103810&gt;=300 and C92544=C111568 and C2851=0)</t>
-  </si>
-  <si>
-    <t>(C15175=0) or (C15175=C17998) or (C15175=1 and C103810&gt;500 and C94631=0) or (C3096=0) or (C3096=Y and C92544=C111568 or (C141405=0) or (C129452C=0)</t>
-  </si>
-  <si>
     <t>(C15175=0) or (C15175=C17998) or (C15175=1 and  C103810&gt;=500) and ((C15175=1 and C94631=1 and C92544&lt;50) or (C15175=1 and C94631=0 and C92544&lt;25000)) and (C947=0) and (C1428=0)</t>
   </si>
   <si>
@@ -4084,9 +4063,6 @@
   </si>
   <si>
     <t>(C14139=0) or (C15175=0) or (C15175=C17998) or (C15175=Y and  C103810&gt;400 and C94631=0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(C15175=0 or C15175=C17998) and C2851=0) </t>
   </si>
   <si>
     <t xml:space="preserve">C15175=0 or C15175=C17998 and (C2851=0 and C14139=0)
@@ -4132,24 +4108,15 @@
     <t>(C15175=0) or (C15175=C17998) or (C15175=1 and C4991=0 and C115935=1 and C92544&gt;=200 and C94631=1 and C97366=0 and C97360=0 and  C1428=0 and C947=0)</t>
   </si>
   <si>
-    <t>C15175=0 or C15175=C17998 or ((C15175=1 and (C111373=0 or  C111374=0))</t>
-  </si>
-  <si>
     <t>C15175=0 or C15175=C17998 or (C15175=1 and C103810&gt;=250 and C2851=0 and C111373=0)</t>
   </si>
   <si>
-    <t>C15175=0 or C15175=C17998 or (C15175=1 and C103810&gt;=200) and C94631=1)</t>
-  </si>
-  <si>
     <t>C15175=0 or C15175=C17998 or (C15175=1 and C103810&gt;250)</t>
   </si>
   <si>
     <t>C15175=0 or C15175=C17998 or (C15175=1 and C103810&gt;=200 and C94631=1)</t>
   </si>
   <si>
-    <t>C15175=0 or C15175=C17998 or (C15175=1 and  C103810 and ((C94631=0) or (C94631=1 and C97366=0)) and C2851=0 and C115935=1</t>
-  </si>
-  <si>
     <t>C15175=0 or C15175=C17998 or (C15175=1 and ((C94631=0) or (C94631=1 and C111373=0 and C103810=AC63350)))</t>
   </si>
   <si>
@@ -4159,9 +4126,6 @@
     <t>C15175=0 or C15175=C17998 or (C15175=1 and C103810&gt;=200)</t>
   </si>
   <si>
-    <t>C15175=0 or C15175=C17998 or (C15175=1 and C2851=0 and C103810&gt;=200 and C94631=1 and C947=0 and C1609=0 and 3-drugs-in-1 pill=0)</t>
-  </si>
-  <si>
     <t>C15175=0 or C15175=C17998 or (C15175=1 and C103810&gt;=250 and C94631=1)</t>
   </si>
   <si>
@@ -4186,9 +4150,6 @@
     <t>(C15175=0) or (C15175=Y and C103810&gt;=250} and C2851=0)</t>
   </si>
   <si>
-    <t>C15175=0 or C15175=C17998 or {C15175=1 and C2851=0 and  C103810&gt;=200 and (C94631=0 or (C94631=1 and C92544&lt;200)) and C947=0) and  C103810&gt;=300}</t>
-  </si>
-  <si>
     <t>(C15175=0) or (C15175=Y and C94631=0 and  C103810&gt;250) and (C15175=Y and C94631=Y and  C103810&gt;250)</t>
   </si>
   <si>
@@ -4207,20 +4168,55 @@
     <t>C15175=0 or C15175=C17998 or (C15175=1 and C103810&gt;=250 and TS_HIV=1 and C947=0 and C115935=1 and C2851=0)</t>
   </si>
   <si>
-    <t>C15175=0 or C15175=C17998 or (C15175=1 and C94631=1 C94631&gt;=4 and C92544&lt;200)</t>
-  </si>
-  <si>
     <t>C15175=0 or C15175=C17998 or (C15175=1 and C2851=0 and C92544=C111568 and TS_HIV=1)</t>
   </si>
   <si>
     <t>C15175=0 or C15175=C17998 or (C15175=1 and C94631=1 and C92544&lt;50 and C103810&gt;250 and C3289=0 and C3184=1)</t>
   </si>
   <si>
-    <t xml:space="preserve">C15175=0 or C15175=C17998 or (C15175=1 and C94631=1 and Cytochrome-P450-2C19-Inducer=0 and Cytochrome-P450-2C19-Inhibotor=0 and C111373=0 and C111374=0 and C97453=0 and C97366=0 and C97360=0) and C92544&lt;1000))
-</t>
-  </si>
-  <si>
     <t>C15175=0 or C15175=C17998 or (C15175=1 and  C103810&gt;=350 and C2851=0 and C947=0 and C1428=0)</t>
+  </si>
+  <si>
+    <t>(C15175=0) or (C15175=C17998) or (C15175=1 and C103810&gt;499 and C92544&lt;50)</t>
+  </si>
+  <si>
+    <t>(C15175=0) or (C15175=C17998 or C15175=1 and C94631=0) or (C15175=1 and C2851=0)</t>
+  </si>
+  <si>
+    <t>(C15175=0) or (C15175=C17998) or (C15175=1 and C94631=0) or (C15175=1 and C94631=1 and C111373=0 and  C103810&gt;=300 and C92544=C111568 and C2851=0)</t>
+  </si>
+  <si>
+    <t>(C15175=0) or (C15175=C17998) or (C15175=1 and C103810&gt;500 and C94631=0) or (C3096=0) or (C3096=1 and C92544=C111568 or C141405=0 or C129452C=0)</t>
+  </si>
+  <si>
+    <t>C15175=0 or C15175=C17998 or (C15175=1 and (C111373=0 or  C111374=0))</t>
+  </si>
+  <si>
+    <t>C15175=0 or C15175=C17998 or (C15175=1 and C103810&gt;=200) and C94631=1</t>
+  </si>
+  <si>
+    <t>C15175=0 or C15175=C17998 or (C15175=1 and  C103810&gt;=200) and C94631=1</t>
+  </si>
+  <si>
+    <t>C15175=0 or C15175=C17998 or (C15175=1 and  C103810 and C94631=0) or (C94631=1 and C97366=0) and C2851=0 and C115935=1</t>
+  </si>
+  <si>
+    <t>C15175=0 or C15175=C17998 or (C15175=1 and C2851=0 and C103810&gt;=200 and C94631=1 and C947=0 and C1609=0 and C909025=0)</t>
+  </si>
+  <si>
+    <t>C15175=0 or C15175=C17998 or (C15175=1 and C2851=0 and  C103810&gt;=200 and (C94631=0 or (C94631=1 and C92544&lt;200)) and C947=0 and  C103810&gt;=300)</t>
+  </si>
+  <si>
+    <t>C15175=0 or C15175=C17998 or (C15175=1 and C94631=1 and C94631&gt;=4 and C92544&lt;200)</t>
+  </si>
+  <si>
+    <t>C15175=0 or C15175=C17998 or (C15175=1 and C94631=1 and C909026=0 and C909027=0 and C111373=0 and C111374=0 and C97453=0 and C97366=0 and C97360=0 and C92544&lt;1000)</t>
+  </si>
+  <si>
+    <t>C15175=0 or C15175=C17998 or (C15175=1 and C103810&gt;=350 and C92544&lt;25000 and C94631=1)</t>
+  </si>
+  <si>
+    <t>C15175=0 or C15175=C17998 or C2851=0 or C2851=C17998 or (C15175=1 and C103810&gt;=250 and C92544=C111568)</t>
   </si>
 </sst>
 </file>
@@ -4675,7 +4671,7 @@
   <dimension ref="A1:G343"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H133" sqref="H133"/>
+      <selection activeCell="H273" sqref="H273"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" thickBottom="1"/>
@@ -4969,7 +4965,7 @@
         <v>40</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>1224</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="135.75" thickBot="1">
@@ -5043,7 +5039,7 @@
         <v>50</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="75.75" thickBot="1">
@@ -5094,7 +5090,7 @@
         <v>55</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>1252</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="105.75" thickBot="1">
@@ -5435,7 +5431,7 @@
         <v>85</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="105.75" thickBot="1">
@@ -5481,7 +5477,7 @@
         <v>95</v>
       </c>
       <c r="G44" s="12" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="409.6" thickBot="1">
@@ -5527,7 +5523,7 @@
         <v>106</v>
       </c>
       <c r="G46" s="11" t="s">
-        <v>1253</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="75.75" thickBot="1">
@@ -5606,7 +5602,7 @@
         <v>111</v>
       </c>
       <c r="G51" s="11" t="s">
-        <v>1254</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="300.75" thickBot="1">
@@ -5629,7 +5625,7 @@
         <v>116</v>
       </c>
       <c r="G52" s="11" t="s">
-        <v>1255</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="75.75" thickBot="1">
@@ -5652,7 +5648,7 @@
         <v>121</v>
       </c>
       <c r="G53" s="14" t="s">
-        <v>1256</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="45.75" thickBot="1">
@@ -5768,7 +5764,7 @@
         <v>130</v>
       </c>
       <c r="G60" s="11" t="s">
-        <v>1302</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="105.75" thickBot="1">
@@ -5791,7 +5787,7 @@
         <v>135</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>1257</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="30.75" thickBot="1">
@@ -5939,7 +5935,7 @@
         <v>155</v>
       </c>
       <c r="G69" s="14" t="s">
-        <v>1258</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="70" spans="1:7" ht="45.75" thickBot="1">
@@ -5976,7 +5972,7 @@
         <v>160</v>
       </c>
       <c r="G71" s="14" t="s">
-        <v>1259</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="105.75" thickBot="1">
@@ -6013,7 +6009,7 @@
         <v>165</v>
       </c>
       <c r="G73" s="14" t="s">
-        <v>1260</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="74" spans="1:7" ht="180.75" thickBot="1">
@@ -6036,7 +6032,7 @@
         <v>169</v>
       </c>
       <c r="G74" s="14" t="s">
-        <v>1261</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="60.75" thickBot="1">
@@ -6059,7 +6055,7 @@
         <v>174</v>
       </c>
       <c r="G75" s="14" t="s">
-        <v>1262</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="409.6" thickBot="1">
@@ -6119,7 +6115,7 @@
         <v>185</v>
       </c>
       <c r="G78" s="11" t="s">
-        <v>1263</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="79" spans="1:7" ht="75.75" thickBot="1">
@@ -6179,7 +6175,7 @@
         <v>193</v>
       </c>
       <c r="G81" s="11" t="s">
-        <v>1256</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="82" spans="1:7" ht="60.75" thickBot="1">
@@ -6225,7 +6221,7 @@
         <v>201</v>
       </c>
       <c r="G83" s="11" t="s">
-        <v>1264</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="84" spans="1:7" ht="135.75" thickBot="1">
@@ -6248,7 +6244,7 @@
         <v>206</v>
       </c>
       <c r="G84" s="11" t="s">
-        <v>1265</v>
+        <v>1257</v>
       </c>
     </row>
     <row r="85" spans="1:7" ht="45.75" thickBot="1">
@@ -6285,7 +6281,7 @@
         <v>211</v>
       </c>
       <c r="G86" s="11" t="s">
-        <v>1266</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="87" spans="1:7" ht="75.75" thickBot="1">
@@ -6308,7 +6304,7 @@
         <v>216</v>
       </c>
       <c r="G87" s="11" t="s">
-        <v>1267</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="88" spans="1:7" ht="60.75" thickBot="1">
@@ -6368,7 +6364,7 @@
         <v>225</v>
       </c>
       <c r="G90" s="11" t="s">
-        <v>1268</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="91" spans="1:7" ht="60.75" thickBot="1">
@@ -6414,7 +6410,7 @@
         <v>234</v>
       </c>
       <c r="G92" s="11" t="s">
-        <v>1269</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="93" spans="1:7" ht="60.75" thickBot="1">
@@ -6451,7 +6447,7 @@
         <v>239</v>
       </c>
       <c r="G94" s="11" t="s">
-        <v>1270</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="95" spans="1:7" ht="60.75" thickBot="1">
@@ -6594,7 +6590,7 @@
         <v>260</v>
       </c>
       <c r="G101" s="11" t="s">
-        <v>1250</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="60.75" thickBot="1">
@@ -6617,7 +6613,7 @@
         <v>264</v>
       </c>
       <c r="G102" s="11" t="s">
-        <v>1271</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="75.75" thickBot="1">
@@ -6640,7 +6636,7 @@
         <v>269</v>
       </c>
       <c r="G103" s="11" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="30.75" thickBot="1">
@@ -6714,7 +6710,7 @@
         <v>279</v>
       </c>
       <c r="G107" s="11" t="s">
-        <v>1251</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="108" spans="1:7" ht="60.75" thickBot="1">
@@ -6760,7 +6756,7 @@
         <v>279</v>
       </c>
       <c r="G109" s="11" t="s">
-        <v>1251</v>
+        <v>1247</v>
       </c>
     </row>
     <row r="110" spans="1:7" ht="409.6" thickBot="1">
@@ -6783,7 +6779,7 @@
         <v>292</v>
       </c>
       <c r="G110" s="11" t="s">
-        <v>1272</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="75.75" thickBot="1">
@@ -6843,7 +6839,7 @@
         <v>303</v>
       </c>
       <c r="G113" s="11" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
     </row>
     <row r="114" spans="1:7" ht="90.75" thickBot="1">
@@ -6912,7 +6908,7 @@
         <v>318</v>
       </c>
       <c r="G116" s="11" t="s">
-        <v>1287</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="117" spans="1:7" ht="105.75" thickBot="1">
@@ -7046,7 +7042,7 @@
         <v>335</v>
       </c>
       <c r="G123" s="11" t="s">
-        <v>1288</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="124" spans="1:7" ht="60.75" thickBot="1">
@@ -7115,7 +7111,7 @@
         <v>350</v>
       </c>
       <c r="G126" s="11" t="s">
-        <v>1273</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="135.75" thickBot="1">
@@ -7221,7 +7217,7 @@
         <v>368</v>
       </c>
       <c r="G131" s="11" t="s">
-        <v>1274</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="132" spans="1:7" ht="45.75" thickBot="1">
@@ -7302,7 +7298,7 @@
         <v>382</v>
       </c>
       <c r="G135" s="11" t="s">
-        <v>1275</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="136" spans="1:7" ht="75.75" thickBot="1">
@@ -7339,7 +7335,7 @@
         <v>387</v>
       </c>
       <c r="G137" s="11" t="s">
-        <v>1276</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="138" spans="1:7" ht="60.75" thickBot="1">
@@ -7399,7 +7395,7 @@
         <v>395</v>
       </c>
       <c r="G140" s="11" t="s">
-        <v>1229</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="141" spans="1:7" ht="60.75" thickBot="1">
@@ -7510,7 +7506,7 @@
         <v>408</v>
       </c>
       <c r="G146" s="11" t="s">
-        <v>1289</v>
+        <v>1277</v>
       </c>
     </row>
     <row r="147" spans="1:7" ht="165.75" thickBot="1">
@@ -7579,7 +7575,7 @@
         <v>422</v>
       </c>
       <c r="G149" s="11" t="s">
-        <v>1292</v>
+        <v>1279</v>
       </c>
     </row>
     <row r="150" spans="1:7" ht="135.75" thickBot="1">
@@ -7602,7 +7598,7 @@
         <v>427</v>
       </c>
       <c r="G150" s="11" t="s">
-        <v>1230</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="151" spans="1:7" ht="60.75" thickBot="1">
@@ -7694,7 +7690,7 @@
         <v>446</v>
       </c>
       <c r="G154" s="11" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
     </row>
     <row r="155" spans="1:7" ht="30.75" thickBot="1">
@@ -7805,7 +7801,7 @@
         <v>460</v>
       </c>
       <c r="G160" s="11" t="s">
-        <v>1231</v>
+        <v>1229</v>
       </c>
     </row>
     <row r="161" spans="1:7" ht="150.75" thickBot="1">
@@ -7828,7 +7824,7 @@
         <v>465</v>
       </c>
       <c r="G161" s="11" t="s">
-        <v>1232</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="162" spans="1:7" ht="75.75" thickBot="1">
@@ -7888,7 +7884,7 @@
         <v>473</v>
       </c>
       <c r="G164" s="11" t="s">
-        <v>1233</v>
+        <v>1231</v>
       </c>
     </row>
     <row r="165" spans="1:7" ht="60.75" thickBot="1">
@@ -7957,7 +7953,7 @@
         <v>486</v>
       </c>
       <c r="G167" s="11" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="168" spans="1:7" ht="60.75" thickBot="1">
@@ -8040,7 +8036,7 @@
         <v>498</v>
       </c>
       <c r="G171" s="11" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="172" spans="1:7" ht="75.75" thickBot="1">
@@ -8151,7 +8147,7 @@
         <v>512</v>
       </c>
       <c r="G177" s="11" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="178" spans="1:7" ht="60.75" thickBot="1">
@@ -8211,7 +8207,7 @@
         <v>521</v>
       </c>
       <c r="G180" s="11" t="s">
-        <v>1293</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="181" spans="1:7" ht="60.75" thickBot="1">
@@ -8257,7 +8253,7 @@
         <v>530</v>
       </c>
       <c r="G182" s="11" t="s">
-        <v>1277</v>
+        <v>1267</v>
       </c>
     </row>
     <row r="183" spans="1:7" ht="409.6" thickBot="1">
@@ -8280,7 +8276,7 @@
         <v>535</v>
       </c>
       <c r="G183" s="11" t="s">
-        <v>1294</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="184" spans="1:7" ht="409.6" thickBot="1">
@@ -8303,7 +8299,7 @@
         <v>540</v>
       </c>
       <c r="G184" s="11" t="s">
-        <v>1278</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="185" spans="1:7" ht="135.75" thickBot="1">
@@ -8326,7 +8322,7 @@
         <v>545</v>
       </c>
       <c r="G185" s="11" t="s">
-        <v>1279</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="186" spans="1:7" ht="90.75" thickBot="1">
@@ -8372,7 +8368,7 @@
         <v>554</v>
       </c>
       <c r="G187" s="11" t="s">
-        <v>1290</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="188" spans="1:7" ht="409.6" thickBot="1">
@@ -8395,7 +8391,7 @@
         <v>559</v>
       </c>
       <c r="G188" s="11" t="s">
-        <v>1280</v>
+        <v>1269</v>
       </c>
     </row>
     <row r="189" spans="1:7" ht="105.75" thickBot="1">
@@ -8418,7 +8414,7 @@
         <v>564</v>
       </c>
       <c r="G189" s="11" t="s">
-        <v>1281</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="190" spans="1:7" ht="345.75" thickBot="1">
@@ -8441,7 +8437,7 @@
         <v>569</v>
       </c>
       <c r="G190" s="11" t="s">
-        <v>1282</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="191" spans="1:7" ht="75.75" thickBot="1">
@@ -8464,7 +8460,7 @@
         <v>574</v>
       </c>
       <c r="G191" s="11" t="s">
-        <v>1283</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="192" spans="1:7" ht="120.75" thickBot="1">
@@ -8487,7 +8483,7 @@
         <v>579</v>
       </c>
       <c r="G192" s="11" t="s">
-        <v>1284</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="193" spans="1:7" ht="375.75" thickBot="1">
@@ -8510,7 +8506,7 @@
         <v>584</v>
       </c>
       <c r="G193" s="11" t="s">
-        <v>1295</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="194" spans="1:7" ht="30.75" thickBot="1">
@@ -8598,7 +8594,7 @@
         <v>594</v>
       </c>
       <c r="G198" s="11" t="s">
-        <v>1285</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="199" spans="1:7" ht="409.6" thickBot="1">
@@ -8621,7 +8617,7 @@
         <v>599</v>
       </c>
       <c r="G199" s="11" t="s">
-        <v>1286</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="200" spans="1:7" ht="90.75" thickBot="1">
@@ -8769,7 +8765,7 @@
         <v>615</v>
       </c>
       <c r="G207" s="11" t="s">
-        <v>1296</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="208" spans="1:7" ht="90.75" thickBot="1">
@@ -8907,7 +8903,7 @@
         <v>644</v>
       </c>
       <c r="G213" s="11" t="s">
-        <v>1291</v>
+        <v>1297</v>
       </c>
     </row>
     <row r="214" spans="1:7" ht="75.75" thickBot="1">
@@ -8990,7 +8986,7 @@
         <v>655</v>
       </c>
       <c r="G217" s="11" t="s">
-        <v>1234</v>
+        <v>1232</v>
       </c>
     </row>
     <row r="218" spans="1:7" ht="180.75" thickBot="1">
@@ -9184,7 +9180,7 @@
         <v>680</v>
       </c>
       <c r="G227" s="11" t="s">
-        <v>1235</v>
+        <v>1233</v>
       </c>
     </row>
     <row r="228" spans="1:7" ht="409.6" thickBot="1">
@@ -9207,7 +9203,7 @@
         <v>685</v>
       </c>
       <c r="G228" s="11" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
     </row>
     <row r="229" spans="1:7" ht="45.75" thickBot="1">
@@ -9281,7 +9277,7 @@
         <v>695</v>
       </c>
       <c r="G232" s="11" t="s">
-        <v>1297</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="233" spans="1:7" ht="45.75" thickBot="1">
@@ -9341,7 +9337,7 @@
         <v>703</v>
       </c>
       <c r="G235" s="11" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
     </row>
     <row r="236" spans="1:7" ht="409.6" thickBot="1">
@@ -9364,7 +9360,7 @@
         <v>708</v>
       </c>
       <c r="G236" s="11" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
     </row>
     <row r="237" spans="1:7" ht="75.75" thickBot="1">
@@ -9433,7 +9429,7 @@
         <v>722</v>
       </c>
       <c r="G239" s="11" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="240" spans="1:7" ht="90.75" thickBot="1">
@@ -9553,7 +9549,7 @@
         <v>740</v>
       </c>
       <c r="G245" s="11" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
     </row>
     <row r="246" spans="1:7" ht="270.75" thickBot="1">
@@ -9576,7 +9572,7 @@
         <v>745</v>
       </c>
       <c r="G246" s="11" t="s">
-        <v>1299</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="247" spans="1:7" ht="45.75" thickBot="1">
@@ -9678,7 +9674,7 @@
         <v>754</v>
       </c>
       <c r="G252" s="11" t="s">
-        <v>1300</v>
+        <v>1286</v>
       </c>
     </row>
     <row r="253" spans="1:7" ht="60.75" thickBot="1">
@@ -9775,7 +9771,7 @@
         <v>769</v>
       </c>
       <c r="G257" s="11" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="258" spans="1:7" ht="45.75" thickBot="1">
@@ -9858,7 +9854,7 @@
         <v>782</v>
       </c>
       <c r="G261" s="11" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="262" spans="1:7" ht="60.75" thickBot="1">
@@ -10048,7 +10044,7 @@
         <v>798</v>
       </c>
       <c r="G272" s="11" t="s">
-        <v>1247</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="273" spans="1:7" ht="285.75" thickBot="1">
@@ -10071,7 +10067,7 @@
         <v>803</v>
       </c>
       <c r="G273" s="11" t="s">
-        <v>1248</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="274" spans="1:7" ht="60.75" thickBot="1">
@@ -10108,7 +10104,7 @@
         <v>808</v>
       </c>
       <c r="G275" s="11" t="s">
-        <v>1249</v>
+        <v>1245</v>
       </c>
     </row>
     <row r="276" spans="1:7" customFormat="1" ht="15"/>
@@ -10194,7 +10190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>